<commit_message>
data updates - cso data
still don’t understand why the logos for some companies - e.g. nielsen
and chrysler - aren’t showing up event hough they exist
</commit_message>
<xml_diff>
--- a/www/data/iday14-companyInfo-succinct.xlsx
+++ b/www/data/iday14-companyInfo-succinct.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="0" windowWidth="22520" windowHeight="17560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="4340" yWindow="0" windowWidth="22520" windowHeight="17560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="majors+positions" sheetId="1" r:id="rId1"/>
@@ -2930,7 +2930,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -2940,6 +2940,25 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3056,7 +3075,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="34">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -3066,6 +3085,25 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -3402,8 +3440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="U51" sqref="A1:U51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6027,7 +6065,7 @@
   <dimension ref="A1:V51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U51" sqref="A1:U51"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8747,7 +8785,7 @@
   <dimension ref="A1:T60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>